<commit_message>
add kpop question in list
</commit_message>
<xml_diff>
--- a/Questions/AllQuestionList.xlsx
+++ b/Questions/AllQuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780E1B73-C8F3-174B-9EE0-45B97CFFF452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2320AF26-2FB2-544A-959C-08A2A7C0F3C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="28300" windowHeight="17040" xr2:uid="{D7A6323F-AAD6-E248-9CA7-6632C1438016}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,14 @@
   </si>
   <si>
     <t>들려오는 곡이 나온 '애니메이션의 이름을' 입력해 주세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도전! 한국 가요 마스터! (난이도 중)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>들려오는 곡의 '제목을' 입력해 주세요!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -436,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831136E3-9C95-8B4F-B26F-E9CDC5B3AA45}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -489,6 +497,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add question && server
</commit_message>
<xml_diff>
--- a/Questions/AllQuestionList.xlsx
+++ b/Questions/AllQuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7979E298-1FC3-8D46-992D-E7B5AAA2BED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1477621B-91A0-994D-B492-C43873377D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="960" windowWidth="28300" windowHeight="17040" xr2:uid="{D7A6323F-AAD6-E248-9CA7-6632C1438016}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>title</t>
   </si>
@@ -77,7 +77,11 @@
     <t>제시되는 노래를 듣고 애니메이션의 '제목을' 입력해주세요!</t>
   </si>
   <si>
-    <t>드라마 OST로 안방극장 탐험(</t>
+    <t>드라마 OST로 안방극장 탐험(난이도 중)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>들려오는 곡이 나온 '드라마의 이름'을 입력해 주세요!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -455,7 +459,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -525,6 +529,9 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="1"/>

</xml_diff>